<commit_message>
Created clustering. finalised code
</commit_message>
<xml_diff>
--- a/Renewable.xlsx
+++ b/Renewable.xlsx
@@ -21,11 +21,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t xml:space="preserve">Series Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Series Code</t>
+  </si>
+  <si>
     <t xml:space="preserve">Country Name</t>
   </si>
   <si>
@@ -125,21 +128,21 @@
     <t xml:space="preserve">Renewable energy consumption (% of total final energy consumption)</t>
   </si>
   <si>
+    <t xml:space="preserve">EG.FEC.RNEW.ZS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IND</t>
+  </si>
+  <si>
     <t xml:space="preserve">United Kingdom</t>
   </si>
   <si>
     <t xml:space="preserve">GBR</t>
   </si>
   <si>
-    <t xml:space="preserve">India</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t xml:space="preserve">Code</t>
   </si>
   <si>
@@ -165,9 +168,6 @@
   </si>
   <si>
     <t xml:space="preserve">License URL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EG.FEC.RNEW.ZS</t>
   </si>
   <si>
     <t xml:space="preserve">CC BY-4.0</t>
@@ -265,12 +265,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -299,341 +295,343 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AH7"/>
+  <dimension ref="A1:AH8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="7:7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="8:8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="0" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="AH1" s="0" t="s">
         <v>33</v>
       </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>58.652858348278</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>57.6047933357271</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>57.2305674845727</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>56.9833633428903</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>55.5571874605853</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>54.4841170038941</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>53.767409699754</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>52.4880731033173</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>52.7122557076625</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>51.7172937036599</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>46.88</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>47.11</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>45.75</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>45.63</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <v>44.92</v>
+      </c>
+      <c r="T2" s="0" t="n">
+        <v>44.16</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <v>43.16</v>
+      </c>
+      <c r="V2" s="0" t="n">
+        <v>41.53</v>
+      </c>
+      <c r="W2" s="0" t="n">
+        <v>39.37</v>
+      </c>
+      <c r="X2" s="0" t="n">
+        <v>37.41</v>
+      </c>
+      <c r="Y2" s="0" t="n">
+        <v>36.16</v>
+      </c>
+      <c r="Z2" s="0" t="n">
+        <v>35.01</v>
+      </c>
+      <c r="AA2" s="0" t="n">
+        <v>34.75</v>
+      </c>
+      <c r="AB2" s="0" t="n">
+        <v>34.85</v>
+      </c>
+      <c r="AC2" s="0" t="n">
+        <v>33.85</v>
+      </c>
+      <c r="AD2" s="0" t="n">
+        <v>33.4</v>
+      </c>
+      <c r="AE2" s="0" t="n">
+        <v>33.02</v>
+      </c>
+      <c r="AF2" s="0" t="n">
+        <v>32.41</v>
+      </c>
+      <c r="AG2" s="0" t="n">
+        <v>32.82</v>
+      </c>
+      <c r="AH2" s="0" t="n">
+        <v>32.93</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="C3" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="0" t="n">
         <v>0.651133978423517</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="F3" s="0" t="n">
         <v>0.608264131136578</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="G3" s="0" t="n">
         <v>0.840737795568959</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="H3" s="0" t="n">
         <v>0.775204971316571</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="I3" s="0" t="n">
         <v>1.02142848392085</v>
       </c>
-      <c r="I2" s="1" t="n">
+      <c r="J3" s="0" t="n">
         <v>1.06022909884603</v>
       </c>
-      <c r="J2" s="1" t="n">
+      <c r="K3" s="0" t="n">
         <v>0.943586897127666</v>
       </c>
-      <c r="K2" s="1" t="n">
+      <c r="L3" s="0" t="n">
         <v>1.02847968902927</v>
       </c>
-      <c r="L2" s="1" t="n">
+      <c r="M3" s="0" t="n">
         <v>1.02970432391514</v>
       </c>
-      <c r="M2" s="1" t="n">
+      <c r="N3" s="0" t="n">
         <v>0.948917657048062</v>
       </c>
-      <c r="N2" s="1" t="n">
+      <c r="O3" s="0" t="n">
         <v>0.96</v>
       </c>
-      <c r="O2" s="1" t="n">
+      <c r="P3" s="0" t="n">
         <v>0.85</v>
       </c>
-      <c r="P2" s="1" t="n">
+      <c r="Q3" s="0" t="n">
         <v>0.97</v>
       </c>
-      <c r="Q2" s="1" t="n">
+      <c r="R3" s="0" t="n">
         <v>0.93</v>
       </c>
-      <c r="R2" s="1" t="n">
+      <c r="S3" s="0" t="n">
         <v>1.14</v>
       </c>
-      <c r="S2" s="1" t="n">
+      <c r="T3" s="0" t="n">
         <v>1.35</v>
       </c>
-      <c r="T2" s="1" t="n">
+      <c r="U3" s="0" t="n">
         <v>1.55</v>
       </c>
-      <c r="U2" s="1" t="n">
+      <c r="V3" s="0" t="n">
         <v>1.84</v>
       </c>
-      <c r="V2" s="1" t="n">
+      <c r="W3" s="0" t="n">
         <v>2.79</v>
       </c>
-      <c r="W2" s="1" t="n">
+      <c r="X3" s="0" t="n">
         <v>3.38</v>
       </c>
-      <c r="X2" s="1" t="n">
+      <c r="Y3" s="0" t="n">
         <v>3.67</v>
       </c>
-      <c r="Y2" s="1" t="n">
+      <c r="Z3" s="0" t="n">
         <v>4.44</v>
       </c>
-      <c r="Z2" s="1" t="n">
+      <c r="AA3" s="0" t="n">
         <v>4.77</v>
       </c>
-      <c r="AA2" s="1" t="n">
+      <c r="AB3" s="0" t="n">
         <v>6.02</v>
       </c>
-      <c r="AB2" s="1" t="n">
+      <c r="AC3" s="0" t="n">
         <v>7.36</v>
       </c>
-      <c r="AC2" s="1" t="n">
+      <c r="AD3" s="0" t="n">
         <v>8.61</v>
       </c>
-      <c r="AD2" s="1" t="n">
+      <c r="AE3" s="0" t="n">
         <v>8.6</v>
       </c>
-      <c r="AE2" s="1" t="n">
+      <c r="AF3" s="0" t="n">
         <v>9.7</v>
       </c>
-      <c r="AF2" s="1" t="n">
+      <c r="AG3" s="0" t="n">
         <v>10.99</v>
       </c>
-      <c r="AG2" s="1" t="n">
+      <c r="AH3" s="0" t="n">
         <v>12.24</v>
       </c>
-      <c r="AH2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>58.652858348278</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>57.6047933357271</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>57.2305674845727</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>56.9833633428903</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <v>55.5571874605853</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>54.4841170038941</v>
-      </c>
-      <c r="J3" s="1" t="n">
-        <v>53.767409699754</v>
-      </c>
-      <c r="K3" s="1" t="n">
-        <v>52.4880731033173</v>
-      </c>
-      <c r="L3" s="1" t="n">
-        <v>52.7122557076625</v>
-      </c>
-      <c r="M3" s="1" t="n">
-        <v>51.7172937036599</v>
-      </c>
-      <c r="N3" s="1" t="n">
-        <v>46.88</v>
-      </c>
-      <c r="O3" s="1" t="n">
-        <v>47.11</v>
-      </c>
-      <c r="P3" s="1" t="n">
-        <v>45.75</v>
-      </c>
-      <c r="Q3" s="1" t="n">
-        <v>45.63</v>
-      </c>
-      <c r="R3" s="1" t="n">
-        <v>44.92</v>
-      </c>
-      <c r="S3" s="1" t="n">
-        <v>44.16</v>
-      </c>
-      <c r="T3" s="1" t="n">
-        <v>43.16</v>
-      </c>
-      <c r="U3" s="1" t="n">
-        <v>41.53</v>
-      </c>
-      <c r="V3" s="1" t="n">
-        <v>39.37</v>
-      </c>
-      <c r="W3" s="1" t="n">
-        <v>37.41</v>
-      </c>
-      <c r="X3" s="1" t="n">
-        <v>36.16</v>
-      </c>
-      <c r="Y3" s="1" t="n">
-        <v>35.01</v>
-      </c>
-      <c r="Z3" s="1" t="n">
-        <v>34.75</v>
-      </c>
-      <c r="AA3" s="1" t="n">
-        <v>34.85</v>
-      </c>
-      <c r="AB3" s="1" t="n">
-        <v>33.85</v>
-      </c>
-      <c r="AC3" s="1" t="n">
-        <v>33.4</v>
-      </c>
-      <c r="AD3" s="1" t="n">
-        <v>33.02</v>
-      </c>
-      <c r="AE3" s="1" t="n">
-        <v>32.41</v>
-      </c>
-      <c r="AF3" s="1" t="n">
-        <v>32.82</v>
-      </c>
-      <c r="AG3" s="1" t="n">
-        <v>32.93</v>
-      </c>
-      <c r="AH3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="2"/>
-      <c r="D7" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
+      <c r="B7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -653,70 +651,70 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="7:7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="8:8 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="2" style="1" width="50.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="2" style="0" width="50.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Graphs now being saved as png files, multiple changes for graphs, Added more comments
</commit_message>
<xml_diff>
--- a/Renewable.xlsx
+++ b/Renewable.xlsx
@@ -131,16 +131,16 @@
     <t xml:space="preserve">EG.FEC.RNEW.ZS</t>
   </si>
   <si>
+    <t xml:space="preserve">United Kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBR</t>
+  </si>
+  <si>
     <t xml:space="preserve">India</t>
   </si>
   <si>
     <t xml:space="preserve">IND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United Kingdom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GBR</t>
   </si>
   <si>
     <t xml:space="preserve">Code</t>
@@ -265,8 +265,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -297,339 +301,335 @@
   </sheetPr>
   <dimension ref="A1:AH8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="8:8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="0" t="s">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="0" t="s">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="0" t="s">
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="0" t="s">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
+        <v>0.651133978423517</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0.608264131136578</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>0.840737795568959</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>0.775204971316571</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>1.02142848392085</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>1.06022909884603</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>0.943586897127666</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>1.02847968902927</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>1.02970432391514</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>0.948917657048062</v>
+      </c>
+      <c r="O2" s="1" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="Q2" s="1" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="S2" s="1" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="T2" s="1" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="U2" s="1" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="V2" s="1" t="n">
+        <v>1.84</v>
+      </c>
+      <c r="W2" s="1" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="X2" s="1" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="Y2" s="1" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="Z2" s="1" t="n">
+        <v>4.44</v>
+      </c>
+      <c r="AA2" s="1" t="n">
+        <v>4.77</v>
+      </c>
+      <c r="AB2" s="1" t="n">
+        <v>6.02</v>
+      </c>
+      <c r="AC2" s="1" t="n">
+        <v>7.36</v>
+      </c>
+      <c r="AD2" s="1" t="n">
+        <v>8.61</v>
+      </c>
+      <c r="AE2" s="1" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="AF2" s="1" t="n">
+        <v>9.7</v>
+      </c>
+      <c r="AG2" s="1" t="n">
+        <v>10.99</v>
+      </c>
+      <c r="AH2" s="1" t="n">
+        <v>12.24</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="1" t="n">
         <v>58.652858348278</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>57.6047933357271</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>57.2305674845727</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>56.9833633428903</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I3" s="1" t="n">
         <v>55.5571874605853</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J3" s="1" t="n">
         <v>54.4841170038941</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K3" s="1" t="n">
         <v>53.767409699754</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="L3" s="1" t="n">
         <v>52.4880731033173</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M3" s="1" t="n">
         <v>52.7122557076625</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="N3" s="1" t="n">
         <v>51.7172937036599</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="O3" s="1" t="n">
         <v>46.88</v>
       </c>
-      <c r="P2" s="0" t="n">
+      <c r="P3" s="1" t="n">
         <v>47.11</v>
       </c>
-      <c r="Q2" s="0" t="n">
+      <c r="Q3" s="1" t="n">
         <v>45.75</v>
       </c>
-      <c r="R2" s="0" t="n">
+      <c r="R3" s="1" t="n">
         <v>45.63</v>
       </c>
-      <c r="S2" s="0" t="n">
+      <c r="S3" s="1" t="n">
         <v>44.92</v>
       </c>
-      <c r="T2" s="0" t="n">
+      <c r="T3" s="1" t="n">
         <v>44.16</v>
       </c>
-      <c r="U2" s="0" t="n">
+      <c r="U3" s="1" t="n">
         <v>43.16</v>
       </c>
-      <c r="V2" s="0" t="n">
+      <c r="V3" s="1" t="n">
         <v>41.53</v>
       </c>
-      <c r="W2" s="0" t="n">
+      <c r="W3" s="1" t="n">
         <v>39.37</v>
       </c>
-      <c r="X2" s="0" t="n">
+      <c r="X3" s="1" t="n">
         <v>37.41</v>
       </c>
-      <c r="Y2" s="0" t="n">
+      <c r="Y3" s="1" t="n">
         <v>36.16</v>
       </c>
-      <c r="Z2" s="0" t="n">
+      <c r="Z3" s="1" t="n">
         <v>35.01</v>
       </c>
-      <c r="AA2" s="0" t="n">
+      <c r="AA3" s="1" t="n">
         <v>34.75</v>
       </c>
-      <c r="AB2" s="0" t="n">
+      <c r="AB3" s="1" t="n">
         <v>34.85</v>
       </c>
-      <c r="AC2" s="0" t="n">
+      <c r="AC3" s="1" t="n">
         <v>33.85</v>
       </c>
-      <c r="AD2" s="0" t="n">
+      <c r="AD3" s="1" t="n">
         <v>33.4</v>
       </c>
-      <c r="AE2" s="0" t="n">
+      <c r="AE3" s="1" t="n">
         <v>33.02</v>
       </c>
-      <c r="AF2" s="0" t="n">
+      <c r="AF3" s="1" t="n">
         <v>32.41</v>
       </c>
-      <c r="AG2" s="0" t="n">
+      <c r="AG3" s="1" t="n">
         <v>32.82</v>
       </c>
-      <c r="AH2" s="0" t="n">
+      <c r="AH3" s="1" t="n">
         <v>32.93</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>0.651133978423517</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>0.608264131136578</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>0.840737795568959</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>0.775204971316571</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>1.02142848392085</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>1.06022909884603</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>0.943586897127666</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>1.02847968902927</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <v>1.02970432391514</v>
-      </c>
-      <c r="N3" s="0" t="n">
-        <v>0.948917657048062</v>
-      </c>
-      <c r="O3" s="0" t="n">
-        <v>0.96</v>
-      </c>
-      <c r="P3" s="0" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="Q3" s="0" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="R3" s="0" t="n">
-        <v>0.93</v>
-      </c>
-      <c r="S3" s="0" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="T3" s="0" t="n">
-        <v>1.35</v>
-      </c>
-      <c r="U3" s="0" t="n">
-        <v>1.55</v>
-      </c>
-      <c r="V3" s="0" t="n">
-        <v>1.84</v>
-      </c>
-      <c r="W3" s="0" t="n">
-        <v>2.79</v>
-      </c>
-      <c r="X3" s="0" t="n">
-        <v>3.38</v>
-      </c>
-      <c r="Y3" s="0" t="n">
-        <v>3.67</v>
-      </c>
-      <c r="Z3" s="0" t="n">
-        <v>4.44</v>
-      </c>
-      <c r="AA3" s="0" t="n">
-        <v>4.77</v>
-      </c>
-      <c r="AB3" s="0" t="n">
-        <v>6.02</v>
-      </c>
-      <c r="AC3" s="0" t="n">
-        <v>7.36</v>
-      </c>
-      <c r="AD3" s="0" t="n">
-        <v>8.61</v>
-      </c>
-      <c r="AE3" s="0" t="n">
-        <v>8.6</v>
-      </c>
-      <c r="AF3" s="0" t="n">
-        <v>9.7</v>
-      </c>
-      <c r="AG3" s="0" t="n">
-        <v>10.99</v>
-      </c>
-      <c r="AH3" s="0" t="n">
-        <v>12.24</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1"/>
-      <c r="D4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -651,70 +651,70 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="8:8 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="2" style="0" width="50.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="2" style="1" width="50.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>